<commit_message>
eliminated one column in Truth file
The last column allows almost unlimited customization; right now it contains two values: paradigm and design; for example FROC paradigm and crossed design. Also allows users to opt out of the new Excel data file format and keep using the old format;
</commit_message>
<xml_diff>
--- a/inst/extdata/CrossedModalitiesData.xlsx
+++ b/inst/extdata/CrossedModalitiesData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28421"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="6220" yWindow="780" windowWidth="20720" windowHeight="12140" activeTab="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4288" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4287" uniqueCount="17">
   <si>
     <t>Case_ID</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>Paradigm</t>
-  </si>
-  <si>
-    <t>Design</t>
   </si>
   <si>
     <t>1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11</t>
@@ -127,8 +124,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -143,11 +142,13 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -79656,10 +79657,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -79667,11 +79668,10 @@
     <col min="1" max="3" width="12.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -79690,11 +79690,8 @@
       <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -79705,19 +79702,16 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -79728,14 +79722,16 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -79746,14 +79742,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -79764,14 +79760,14 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -79782,14 +79778,14 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -79800,14 +79796,14 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -79818,14 +79814,14 @@
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -79836,14 +79832,14 @@
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -79854,14 +79850,14 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -79872,14 +79868,14 @@
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -79890,14 +79886,14 @@
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F12"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -79908,14 +79904,14 @@
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -79926,13 +79922,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -79943,13 +79939,13 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -79960,10 +79956,10 @@
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -79977,10 +79973,10 @@
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -79994,10 +79990,10 @@
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -80011,10 +80007,10 @@
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -80028,10 +80024,10 @@
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -80045,10 +80041,10 @@
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -80062,10 +80058,10 @@
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -80079,10 +80075,10 @@
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -80096,10 +80092,10 @@
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -80113,10 +80109,10 @@
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -80130,10 +80126,10 @@
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -80147,10 +80143,10 @@
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -80164,10 +80160,10 @@
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -80181,10 +80177,10 @@
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -80198,10 +80194,10 @@
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -80215,10 +80211,10 @@
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -80232,10 +80228,10 @@
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -80249,10 +80245,10 @@
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -80266,10 +80262,10 @@
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -80283,10 +80279,10 @@
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -80300,10 +80296,10 @@
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -80317,10 +80313,10 @@
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -80334,10 +80330,10 @@
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -80351,10 +80347,10 @@
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -80368,10 +80364,10 @@
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -80385,10 +80381,10 @@
         <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -80402,10 +80398,10 @@
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -80419,10 +80415,10 @@
         <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -80436,10 +80432,10 @@
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -80453,10 +80449,10 @@
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -80470,10 +80466,10 @@
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -80487,10 +80483,10 @@
         <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -80504,10 +80500,10 @@
         <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -80521,10 +80517,10 @@
         <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -80538,10 +80534,10 @@
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -80555,10 +80551,10 @@
         <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -80572,10 +80568,10 @@
         <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -80589,10 +80585,10 @@
         <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -80606,10 +80602,10 @@
         <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -80623,10 +80619,10 @@
         <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -80640,10 +80636,10 @@
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -80657,10 +80653,10 @@
         <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -80674,10 +80670,10 @@
         <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -80691,10 +80687,10 @@
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -80708,10 +80704,10 @@
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -80725,10 +80721,10 @@
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -80742,10 +80738,10 @@
         <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -80759,10 +80755,10 @@
         <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -80776,10 +80772,10 @@
         <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -80793,10 +80789,10 @@
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -80810,10 +80806,10 @@
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -80827,10 +80823,10 @@
         <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -80844,10 +80840,10 @@
         <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -80861,10 +80857,10 @@
         <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -80878,10 +80874,10 @@
         <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -80895,10 +80891,10 @@
         <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -80912,10 +80908,10 @@
         <v>0</v>
       </c>
       <c r="D72" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -80929,10 +80925,10 @@
         <v>0</v>
       </c>
       <c r="D73" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -80946,10 +80942,10 @@
         <v>0</v>
       </c>
       <c r="D74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -80963,10 +80959,10 @@
         <v>0</v>
       </c>
       <c r="D75" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -80980,10 +80976,10 @@
         <v>0</v>
       </c>
       <c r="D76" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -80997,10 +80993,10 @@
         <v>0</v>
       </c>
       <c r="D77" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -81014,10 +81010,10 @@
         <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -81031,10 +81027,10 @@
         <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -81048,10 +81044,10 @@
         <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -81065,10 +81061,10 @@
         <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>